<commit_message>
0.9.5 - Added many features. Close parity with older IRAP 2012, visual basic 6 implementation.
1. Added option for block order selection via the dialogue box.
2. Added autorespone monkey
3. Added option for image stimuli.
4. Added Colored text for pre block rules.
5. Added option for moving response options.
6. Tidied up post block text and locations.
7. Added warning level logging
8. Seperated the block layout and stimuli excel files. This allows for
an arbitrary number of exemplars for each stimulus category.
9. Commented out the saving of median latency and % accuracy data to
the csv file, as it was causing problems in reading the file into R.
</commit_message>
<xml_diff>
--- a/stimuli.xlsx
+++ b/stimuli.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="26330"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="26819"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14880" tabRatio="500"/>
@@ -22,94 +22,64 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="17">
   <si>
-    <t>target</t>
+    <t>categoryA_stimuli</t>
   </si>
   <si>
-    <t>label</t>
+    <t>categoryB_stimuli</t>
   </si>
   <si>
-    <t>responseOption1</t>
+    <t>categoryC_stimuli</t>
   </si>
   <si>
-    <t>responseOption2</t>
+    <t>categoryD_stimuli</t>
   </si>
   <si>
-    <t>trialType</t>
+    <t>categoryA_image_stimuli</t>
   </si>
   <si>
-    <t>d</t>
+    <t>categoryB_image_stimuli</t>
   </si>
   <si>
-    <t>k</t>
+    <t>categoryC_image_stimuli</t>
   </si>
   <si>
-    <t>True</t>
+    <t>categoryD_image_stimuli</t>
   </si>
   <si>
-    <t>False</t>
+    <t>blank.png</t>
   </si>
   <si>
-    <t>allowAns2</t>
+    <t>happy</t>
   </si>
   <si>
-    <t>allowAns1</t>
+    <t>friendly</t>
   </si>
   <si>
-    <t>correctAns1</t>
+    <t>pretty</t>
   </si>
   <si>
-    <t>correctAns2</t>
+    <t>good</t>
   </si>
   <si>
-    <t>I am</t>
+    <t>pain</t>
   </si>
   <si>
-    <t>Others people are</t>
+    <t>mean</t>
   </si>
   <si>
-    <t xml:space="preserve">Loyal  </t>
+    <t>hostile</t>
   </si>
   <si>
-    <t>Trustworthy</t>
-  </si>
-  <si>
-    <t>Kind</t>
-  </si>
-  <si>
-    <t>Moral</t>
-  </si>
-  <si>
-    <t>Generous</t>
-  </si>
-  <si>
-    <t>Friendly</t>
-  </si>
-  <si>
-    <t>Manipulative</t>
-  </si>
-  <si>
-    <t>Dishonest</t>
-  </si>
-  <si>
-    <t>Cruel</t>
-  </si>
-  <si>
-    <t>Horrible</t>
-  </si>
-  <si>
-    <t>Selfish</t>
-  </si>
-  <si>
-    <t>Heartless</t>
+    <t>hateful</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -126,41 +96,13 @@
       <color theme="11"/>
       <name val="Verdana"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <name val="Verdana"/>
-    </font>
   </fonts>
-  <fills count="6">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -172,7 +114,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="679">
+  <cellStyleXfs count="713">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -852,31 +794,47 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="679">
+  <cellStyles count="713">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1216,6 +1174,23 @@
     <cellStyle name="Followed Hyperlink" xfId="674" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="676" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="678" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="680" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="682" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="684" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="686" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="688" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="690" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="692" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="694" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="696" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="698" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="700" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="702" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="704" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="706" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="708" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="710" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="712" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1555,6 +1530,23 @@
     <cellStyle name="Hyperlink" xfId="673" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="675" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="677" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="679" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="681" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="683" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="685" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="687" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="689" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="691" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="693" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="695" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="697" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="699" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="701" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="703" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="705" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="707" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="709" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="711" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1882,745 +1874,253 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27:F43"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="20" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" customWidth="1"/>
-    <col min="3" max="3" width="7.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" customWidth="1"/>
-    <col min="7" max="9" width="12.42578125" customWidth="1"/>
+    <col min="1" max="2" width="16" customWidth="1"/>
+    <col min="3" max="3" width="16" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16" customWidth="1"/>
+    <col min="5" max="8" width="19.5703125" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:8">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="B4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="B5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>9</v>
+      <c r="B7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G7" t="s">
+        <v>8</v>
+      </c>
+      <c r="H7" t="s">
+        <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="16">
-      <c r="A2" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="5" t="s">
+    <row r="8" spans="1:8">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="3">
-        <v>1</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>6</v>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" t="s">
+        <v>8</v>
+      </c>
+      <c r="H8" t="s">
+        <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="16">
-      <c r="A3" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="5" t="s">
+    <row r="9" spans="1:8">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="3">
-        <v>1</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="16">
-      <c r="A4" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="3">
-        <v>1</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="16">
-      <c r="A5" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="3">
-        <v>1</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="16">
-      <c r="A6" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="3">
-        <v>1</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="16">
-      <c r="A7" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="3">
-        <v>1</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="16">
-      <c r="A8" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="3">
-        <v>2</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="16">
-      <c r="A9" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="3">
-        <v>2</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="16">
-      <c r="A10" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="3">
-        <v>2</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="16">
-      <c r="A11" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" s="3">
-        <v>2</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="16">
-      <c r="A12" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" s="3">
-        <v>2</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="16">
-      <c r="A13" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" s="3">
-        <v>2</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I13" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="16">
-      <c r="A14" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" s="3">
-        <v>3</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I14" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="16">
-      <c r="A15" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" s="7" t="s">
+      <c r="C9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="3">
-        <v>3</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I15" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="16">
-      <c r="A16" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" s="3">
-        <v>3</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H16" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I16" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="16">
-      <c r="A17" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C17" s="3">
-        <v>3</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I17" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="16">
-      <c r="A18" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C18" s="3">
-        <v>3</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H18" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I18" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="16">
-      <c r="A19" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C19" s="3">
-        <v>3</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I19" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="16">
-      <c r="A20" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B20" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C20" s="3">
-        <v>4</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H20" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I20" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="16">
-      <c r="A21" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B21" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C21" s="3">
-        <v>4</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H21" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I21" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="16">
-      <c r="A22" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B22" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C22" s="3">
-        <v>4</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H22" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I22" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="16">
-      <c r="A23" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B23" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C23" s="3">
-        <v>4</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H23" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I23" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="16">
-      <c r="A24" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C24" s="3">
-        <v>4</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G24" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H24" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I24" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="16">
-      <c r="A25" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B25" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C25" s="3">
-        <v>4</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H25" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I25" s="3" t="s">
-        <v>6</v>
+      <c r="E9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" t="s">
+        <v>8</v>
+      </c>
+      <c r="H9" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updates to R script and readme documentation
</commit_message>
<xml_diff>
--- a/stimuli.xlsx
+++ b/stimuli.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="26819"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="27226"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="14640" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14880" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="trialTypes.csv" sheetId="3" r:id="rId1"/>
@@ -22,31 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="25">
-  <si>
-    <t>categoryA_stimuli</t>
-  </si>
-  <si>
-    <t>categoryB_stimuli</t>
-  </si>
-  <si>
-    <t>categoryC_stimuli</t>
-  </si>
-  <si>
-    <t>categoryD_stimuli</t>
-  </si>
-  <si>
-    <t>categoryA_image_stimuli</t>
-  </si>
-  <si>
-    <t>categoryB_image_stimuli</t>
-  </si>
-  <si>
-    <t>categoryC_image_stimuli</t>
-  </si>
-  <si>
-    <t>categoryD_image_stimuli</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>blank.png</t>
   </si>
@@ -54,49 +30,37 @@
     <t>happy</t>
   </si>
   <si>
-    <t>friendly</t>
-  </si>
-  <si>
-    <t>pretty</t>
-  </si>
-  <si>
-    <t>good</t>
-  </si>
-  <si>
     <t>pain</t>
-  </si>
-  <si>
-    <t>mean</t>
-  </si>
-  <si>
-    <t>hostile</t>
-  </si>
-  <si>
-    <t>hateful</t>
   </si>
   <si>
     <t>daffodil</t>
   </si>
   <si>
-    <t>rose</t>
-  </si>
-  <si>
-    <t>lilly</t>
-  </si>
-  <si>
-    <t>daisy</t>
-  </si>
-  <si>
     <t>spider</t>
   </si>
   <si>
-    <t>wasp</t>
+    <t>labelA_stimuli</t>
   </si>
   <si>
-    <t>maggot</t>
+    <t>labelB_stimuli</t>
   </si>
   <si>
-    <t>bee</t>
+    <t>targetA_stimuli</t>
+  </si>
+  <si>
+    <t>targetB_stimuli</t>
+  </si>
+  <si>
+    <t>labelA_image_stimuli</t>
+  </si>
+  <si>
+    <t>labelB_image_stimuli</t>
+  </si>
+  <si>
+    <t>targetA_image_stimuli</t>
+  </si>
+  <si>
+    <t>targetB_image_stimuli</t>
   </si>
 </sst>
 </file>
@@ -138,8 +102,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="715">
+  <cellStyleXfs count="717">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -860,7 +826,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="715">
+  <cellStyles count="717">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1218,6 +1184,7 @@
     <cellStyle name="Followed Hyperlink" xfId="710" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="712" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="714" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="716" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1575,6 +1542,7 @@
     <cellStyle name="Hyperlink" xfId="709" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="711" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="713" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="715" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1902,10 +1870,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B3" sqref="A3:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -1919,236 +1887,54 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="G1" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="H1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="F2" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="H2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3" t="s">
-        <v>8</v>
-      </c>
-      <c r="H3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G5" t="s">
-        <v>8</v>
-      </c>
-      <c r="H5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G6" t="s">
-        <v>8</v>
-      </c>
-      <c r="H6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F7" t="s">
-        <v>8</v>
-      </c>
-      <c r="G7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" t="s">
-        <v>8</v>
-      </c>
-      <c r="F8" t="s">
-        <v>8</v>
-      </c>
-      <c r="G8" t="s">
-        <v>8</v>
-      </c>
-      <c r="H8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E9" t="s">
-        <v>8</v>
-      </c>
-      <c r="F9" t="s">
-        <v>8</v>
-      </c>
-      <c r="G9" t="s">
-        <v>8</v>
-      </c>
-      <c r="H9" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>